<commit_message>
Deploying to gh-pages from @ eurovibes/bbbalarm@eebfd5ba7cbedf2e00b63c3b5749e4ad7ba35625 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/bbbalarm-bom_0.1.xlsx
+++ b/Fabrication/BoM/bbbalarm-bom_0.1.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="89">
   <si>
     <t>Row</t>
   </si>
@@ -110,7 +110,7 @@
     <t>5</t>
   </si>
   <si>
-    <t>J104 J105</t>
+    <t>J104 J105 J106</t>
   </si>
   <si>
     <t>Conn_01x03</t>
@@ -128,7 +128,7 @@
     <t>JP105 JP106 JP107 JP108</t>
   </si>
   <si>
-    <t>Jumper_NO_Small</t>
+    <t>SolderJumper_2_Open</t>
   </si>
   <si>
     <t>A2</t>
@@ -155,7 +155,7 @@
     <t>8</t>
   </si>
   <si>
-    <t>R101 R102 R103 R104 R105 R106 R107 R108 R109 R110 R111 R112</t>
+    <t>R101 R102 R103 R104 R105 R106 R107 R108 R109 R110 R111 R112 R113</t>
   </si>
   <si>
     <t>R</t>
@@ -167,49 +167,61 @@
     <t>R_0402_1005Metric</t>
   </si>
   <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>SW101 SW102</t>
+  </si>
+  <si>
+    <t>SW_Push_45deg</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>SW_PUSH_6mm</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>U103</t>
+  </si>
+  <si>
+    <t>AT24CS64-SSHM</t>
+  </si>
+  <si>
+    <t>AT24C512C-SSHD-T</t>
+  </si>
+  <si>
+    <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>U101</t>
+  </si>
+  <si>
+    <t>HCPL-263N</t>
+  </si>
+  <si>
+    <t>DIP-8_W7.62mm</t>
+  </si>
+  <si>
     <t>12</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>SW101 SW102</t>
-  </si>
-  <si>
-    <t>SW_Push_45deg</t>
-  </si>
-  <si>
-    <t>Reset</t>
-  </si>
-  <si>
-    <t>SW_PUSH_6mm</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>U103</t>
-  </si>
-  <si>
-    <t>AT24CS64-SSHM</t>
-  </si>
-  <si>
-    <t>AT24C512C-SSHD-T</t>
-  </si>
-  <si>
-    <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>U101</t>
-  </si>
-  <si>
-    <t>HCPL-263N</t>
-  </si>
-  <si>
-    <t>DIP-8_W7.62mm</t>
+    <t>U102</t>
+  </si>
+  <si>
+    <t>SHT35-DIS</t>
+  </si>
+  <si>
+    <t>Sensirion_DFN-8-1EP_2.5x2.5mm_P0.5mm_EP1.1x1.7mm</t>
   </si>
   <si>
     <t>U104</t>
@@ -248,7 +260,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>5.1.9+dfsg1-1~bpo10+1</t>
+    <t>6.0.5+dfsg-1~bpo11+1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -376,34 +388,34 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="justify" wrapText="1"/>
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="justify" wrapText="1"/>
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="justify" wrapText="1"/>
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="justify" wrapText="1"/>
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="justify" wrapText="1"/>
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="justify" wrapText="1"/>
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="justify" wrapText="1"/>
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -426,7 +438,7 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>299049</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>44802</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -742,7 +754,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -765,7 +777,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -777,55 +789,55 @@
     </row>
     <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F2" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="C3" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F3" s="3">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F4" s="3">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -833,16 +845,16 @@
     </row>
     <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F6" s="3">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1034,7 +1046,7 @@
         <v>14</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1101,7 +1113,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" ht="30.0" customHeight="1">
       <c r="A16" s="8" t="s">
         <v>44</v>
       </c>
@@ -1231,33 +1243,65 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J20" s="8" t="s">
+      <c r="B21" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1278,10 +1322,11 @@
     <hyperlink ref="G18" r:id="rId10"/>
     <hyperlink ref="G19" r:id="rId11"/>
     <hyperlink ref="G20" r:id="rId12"/>
+    <hyperlink ref="G21" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId13"/>
+  <drawing r:id="rId14"/>
 </worksheet>
 </file>
 
@@ -1298,17 +1343,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="6" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="7" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ eurovibes/bbbalarm@de7f87e87b92b0efb519c91df71b6fa631b74b0f 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/bbbalarm-bom_0.1.xlsx
+++ b/Fabrication/BoM/bbbalarm-bom_0.1.xlsx
@@ -18,12 +18,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="78">
   <si>
     <t>Row</t>
   </si>
   <si>
-    <t>References</t>
+    <t>Reference</t>
   </si>
   <si>
     <t>Value</t>
@@ -53,6 +53,9 @@
     <t/>
   </si>
   <si>
+    <t>100 nF</t>
+  </si>
+  <si>
     <t>CL05B104KO5NNNC</t>
   </si>
   <si>
@@ -65,16 +68,37 @@
     <t>C_0402_1005Metric</t>
   </si>
   <si>
-    <t>26</t>
+    <t>16V 100nF X7R ±10% 0402  Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
+  </si>
+  <si>
+    <t>24</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>KT-0603R</t>
-  </si>
-  <si>
-    <t>Hubei KENTO Elec</t>
+    <t>1N4004</t>
+  </si>
+  <si>
+    <t>DIOTEC SEMICONDUCTOR</t>
+  </si>
+  <si>
+    <t>D_DO-41_SOD81_P10.16mm_Horizontal</t>
+  </si>
+  <si>
+    <t>rectifying; THT; 400V; 1A; Ammo Pack; Ifsm: 30A; DO41; 1.5us</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>LED green</t>
+  </si>
+  <si>
+    <t>OSG5TA34E4A</t>
+  </si>
+  <si>
+    <t>OPTOSUPPLY</t>
   </si>
   <si>
     <t>C2286</t>
@@ -83,10 +107,25 @@
     <t>LED_D3.0mm</t>
   </si>
   <si>
+    <t>LED diode green 3mm 200~330mcd 20mA 140° THT</t>
+  </si>
+  <si>
     <t>4</t>
   </si>
   <si>
-    <t>3</t>
+    <t>LED red</t>
+  </si>
+  <si>
+    <t>OSR5JA34E4A</t>
+  </si>
+  <si>
+    <t>LED diode red 3mm 68~100mcd 20mA 140° THT</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>1 kΩ</t>
   </si>
   <si>
     <t>0402WGF1001TCE</t>
@@ -101,7 +140,13 @@
     <t>R_0402_1005Metric</t>
   </si>
   <si>
-    <t>5</t>
+    <t>1/16W Thick Film Resistors 50V ±1% ±100ppm/℃ -55℃~+155℃ 1kΩ 0402  Chip Resistor - Surface Mount ROHS</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>AT24C512C-SSHD-T</t>
   </si>
   <si>
     <t>AT24C256C-SSHL-T</t>
@@ -116,6 +161,15 @@
     <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
   </si>
   <si>
+    <t>SOIC-8_150mil  EEPROM ROHS</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>SHT35-DIS</t>
+  </si>
+  <si>
     <t>SHT35-DIS-B2.5KSIC</t>
   </si>
   <si>
@@ -126,6 +180,21 @@
   </si>
   <si>
     <t>Sensirion_DFN-8-1EP_2.5x2.5mm_P0.5mm_EP1.1x1.7mm</t>
+  </si>
+  <si>
+    <t>±1.5% RH 0 ~ 100% RH Humidity, Temperature I²C DFN-8  Humidity Sensors/Temperature and Humidity Sensors ROHS</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>WPMDH1100xx1S</t>
+  </si>
+  <si>
+    <t>TSN 1-2450</t>
+  </si>
+  <si>
+    <t>TRACO POWER</t>
   </si>
   <si>
     <t>KiBot Bill of Materials</t>
@@ -242,13 +311,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE6F9FF"/>
+        <fgColor rgb="FFFFE6B3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFE6B3"/>
+        <fgColor rgb="FFE6F9FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -260,13 +329,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF0FFFF"/>
+        <fgColor rgb="FFFFF0BD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF0BD"/>
+        <fgColor rgb="FFF0FFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -335,8 +404,8 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1984974</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:colOff>1651599</xdr:colOff>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>44802</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -652,7 +721,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -662,19 +731,19 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
     <col min="5" max="5" width="30.7109375" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="53.7109375" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="60.7109375" customWidth="1"/>
     <col min="9" max="9" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -685,27 +754,27 @@
     </row>
     <row r="2" spans="1:9">
       <c r="C2" s="2" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="F2" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="C3" s="2" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="F3" s="3">
         <v>37</v>
@@ -713,13 +782,13 @@
     </row>
     <row r="4" spans="1:9">
       <c r="C4" s="2" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F4" s="3">
         <v>37</v>
@@ -727,13 +796,13 @@
     </row>
     <row r="5" spans="1:9">
       <c r="C5" s="2" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -741,13 +810,13 @@
     </row>
     <row r="6" spans="1:9">
       <c r="C6" s="2" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="F6" s="3">
         <v>37</v>
@@ -782,7 +851,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" ht="30.0" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
@@ -790,140 +859,227 @@
         <v>10</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="D9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="E9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>10</v>
+      <c r="G9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>10</v>
+      <c r="G10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="D11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="6" t="s">
-        <v>10</v>
+      <c r="F11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="8" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>10</v>
+      <c r="H12" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30.0" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" s="6" t="s">
+      <c r="C14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30.0" customHeight="1">
+      <c r="A15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="C15" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -949,18 +1105,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="7" t="s">
-        <v>52</v>
+      <c r="A1" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="6" t="s">
-        <v>54</v>
+      <c r="A3" s="7" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>